<commit_message>
atualização com 2024 e limpeza das categorias de perfil
</commit_message>
<xml_diff>
--- a/documentacao/trab_manual.xlsx
+++ b/documentacao/trab_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOVO\Documents\TCC\novocaged\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD867CF-B950-4663-BEDA-0D132A615F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16147644-2D87-4F45-992E-7DA5526F95EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{8C8F0A4A-4C4E-42EF-BE7B-7BC55AC3B4B5}"/>
   </bookViews>
@@ -1609,11 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD02064-7416-4918-B4F4-C6A329ED0580}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J587"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A164" sqref="A3:A164"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,7 +1650,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>999999</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>111220</v>
       </c>
@@ -5436,7 +5435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>121005</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>122610</v>
       </c>
@@ -5482,7 +5481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>123105</v>
       </c>
@@ -5505,7 +5504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>123110</v>
       </c>
@@ -5528,7 +5527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>123115</v>
       </c>
@@ -5551,7 +5550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>123305</v>
       </c>
@@ -5574,7 +5573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>123405</v>
       </c>
@@ -5597,7 +5596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>123805</v>
       </c>
@@ -5620,7 +5619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>131120</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>141205</v>
       </c>
@@ -5666,7 +5665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>141305</v>
       </c>
@@ -5689,7 +5688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>141405</v>
       </c>
@@ -5712,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>141410</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>141415</v>
       </c>
@@ -5758,7 +5757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>141420</v>
       </c>
@@ -5781,7 +5780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>141505</v>
       </c>
@@ -5804,7 +5803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>141510</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>141605</v>
       </c>
@@ -5850,7 +5849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>141610</v>
       </c>
@@ -5873,7 +5872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>141615</v>
       </c>
@@ -5896,7 +5895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>141710</v>
       </c>
@@ -5919,7 +5918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>141720</v>
       </c>
@@ -5942,7 +5941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>142105</v>
       </c>
@@ -5965,7 +5964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>142110</v>
       </c>
@@ -5988,7 +5987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>142115</v>
       </c>
@@ -6011,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>142205</v>
       </c>
@@ -6034,7 +6033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>142210</v>
       </c>
@@ -6057,7 +6056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>142305</v>
       </c>
@@ -6080,7 +6079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>142315</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>142320</v>
       </c>
@@ -6126,7 +6125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>142325</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>142330</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>142335</v>
       </c>
@@ -6195,7 +6194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>142405</v>
       </c>
@@ -6218,7 +6217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>142410</v>
       </c>
@@ -6241,7 +6240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>142415</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>142505</v>
       </c>
@@ -6287,7 +6286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>142510</v>
       </c>
@@ -6310,7 +6309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>142530</v>
       </c>
@@ -6333,7 +6332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>142705</v>
       </c>
@@ -6356,7 +6355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>201215</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>201225</v>
       </c>
@@ -6402,7 +6401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>202110</v>
       </c>
@@ -6425,7 +6424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>212405</v>
       </c>
@@ -6448,7 +6447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>212410</v>
       </c>
@@ -6471,7 +6470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>212415</v>
       </c>
@@ -6494,7 +6493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>212420</v>
       </c>
@@ -6517,7 +6516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>213205</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>214005</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214010</v>
       </c>
@@ -6586,7 +6585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>214205</v>
       </c>
@@ -6609,7 +6608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>214270</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>214280</v>
       </c>
@@ -6655,7 +6654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>214305</v>
       </c>
@@ -6678,7 +6677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>214315</v>
       </c>
@@ -6701,7 +6700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>214320</v>
       </c>
@@ -6724,7 +6723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>214325</v>
       </c>
@@ -6747,7 +6746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>214405</v>
       </c>
@@ -6770,7 +6769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>214530</v>
       </c>
@@ -6793,7 +6792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>214905</v>
       </c>
@@ -6816,7 +6815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>214910</v>
       </c>
@@ -6839,7 +6838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>214915</v>
       </c>
@@ -6862,7 +6861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>214935</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>215105</v>
       </c>
@@ -6908,7 +6907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>215140</v>
       </c>
@@ -6931,7 +6930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>215205</v>
       </c>
@@ -6954,7 +6953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>215215</v>
       </c>
@@ -6977,7 +6976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>223530</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>223710</v>
       </c>
@@ -7023,7 +7022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>224120</v>
       </c>
@@ -7046,7 +7045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>225140</v>
       </c>
@@ -7069,7 +7068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>241005</v>
       </c>
@@ -7092,7 +7091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>241010</v>
       </c>
@@ -7115,7 +7114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>241040</v>
       </c>
@@ -7138,7 +7137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>251215</v>
       </c>
@@ -7161,7 +7160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>251225</v>
       </c>
@@ -7184,7 +7183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>251605</v>
       </c>
@@ -7207,7 +7206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>252105</v>
       </c>
@@ -7230,7 +7229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>252205</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>252210</v>
       </c>
@@ -7276,7 +7275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>252305</v>
       </c>
@@ -7299,7 +7298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>252405</v>
       </c>
@@ -7322,7 +7321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>252545</v>
       </c>
@@ -7345,7 +7344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>252550</v>
       </c>
@@ -7368,7 +7367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>252705</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>252710</v>
       </c>
@@ -7414,7 +7413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>252715</v>
       </c>
@@ -7437,7 +7436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252720</v>
       </c>
@@ -7460,7 +7459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253115</v>
       </c>
@@ -7483,7 +7482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>253125</v>
       </c>
@@ -7506,7 +7505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>254305</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>261210</v>
       </c>
@@ -7552,7 +7551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>261215</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>262410</v>
       </c>
@@ -7598,7 +7597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>300105</v>
       </c>
@@ -7621,7 +7620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>300305</v>
       </c>
@@ -7644,7 +7643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>314805</v>
       </c>
@@ -7667,7 +7666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>322215</v>
       </c>
@@ -7690,7 +7689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>342105</v>
       </c>
@@ -7713,7 +7712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>342120</v>
       </c>
@@ -7736,7 +7735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>342125</v>
       </c>
@@ -7759,7 +7758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>342205</v>
       </c>
@@ -7782,7 +7781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>342210</v>
       </c>
@@ -7805,7 +7804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>342305</v>
       </c>
@@ -7828,7 +7827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>342310</v>
       </c>
@@ -7851,7 +7850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>342605</v>
       </c>
@@ -7874,7 +7873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>342610</v>
       </c>
@@ -7897,7 +7896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>351305</v>
       </c>
@@ -7920,7 +7919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>351425</v>
       </c>
@@ -7943,7 +7942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>351430</v>
       </c>
@@ -7966,7 +7965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>351505</v>
       </c>
@@ -7989,7 +7988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>351605</v>
       </c>
@@ -8012,7 +8011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>352205</v>
       </c>
@@ -8035,7 +8034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>352310</v>
       </c>
@@ -8058,7 +8057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>353230</v>
       </c>
@@ -8081,7 +8080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>354125</v>
       </c>
@@ -8104,7 +8103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>354130</v>
       </c>
@@ -8127,7 +8126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>354140</v>
       </c>
@@ -8150,7 +8149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>354205</v>
       </c>
@@ -8173,7 +8172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>373140</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>375105</v>
       </c>
@@ -8219,7 +8218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>375110</v>
       </c>
@@ -8242,7 +8241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>391120</v>
       </c>
@@ -8265,7 +8264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>391125</v>
       </c>
@@ -8288,7 +8287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>391130</v>
       </c>
@@ -8311,7 +8310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>391135</v>
       </c>
@@ -8334,7 +8333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>391145</v>
       </c>
@@ -8357,7 +8356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>391205</v>
       </c>
@@ -8380,7 +8379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>391210</v>
       </c>
@@ -8403,7 +8402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>391215</v>
       </c>
@@ -8426,7 +8425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>410105</v>
       </c>
@@ -8449,7 +8448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>410205</v>
       </c>
@@ -8472,7 +8471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>410215</v>
       </c>
@@ -8495,7 +8494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>410235</v>
       </c>
@@ -8518,7 +8517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>410240</v>
       </c>
@@ -8541,7 +8540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>411005</v>
       </c>
@@ -8564,7 +8563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>411010</v>
       </c>
@@ -8587,7 +8586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>411025</v>
       </c>
@@ -8610,7 +8609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>411030</v>
       </c>
@@ -8633,7 +8632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>411045</v>
       </c>
@@ -8656,7 +8655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>412205</v>
       </c>
@@ -8679,7 +8678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>413105</v>
       </c>
@@ -8702,7 +8701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>413110</v>
       </c>
@@ -8725,7 +8724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>413115</v>
       </c>
@@ -8748,7 +8747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>413210</v>
       </c>
@@ -8771,7 +8770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>414105</v>
       </c>
@@ -8794,7 +8793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>414110</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>414115</v>
       </c>
@@ -8840,7 +8839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>414125</v>
       </c>
@@ -8863,7 +8862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>414135</v>
       </c>
@@ -8886,7 +8885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>414140</v>
       </c>
@@ -8909,7 +8908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>414210</v>
       </c>
@@ -8932,7 +8931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>414215</v>
       </c>
@@ -8955,7 +8954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>415210</v>
       </c>
@@ -8978,7 +8977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>420105</v>
       </c>
@@ -9001,7 +9000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>420110</v>
       </c>
@@ -9024,7 +9023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>420135</v>
       </c>
@@ -9047,7 +9046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>421105</v>
       </c>
@@ -9070,7 +9069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>421125</v>
       </c>
@@ -9093,7 +9092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>421305</v>
       </c>
@@ -9116,7 +9115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>421310</v>
       </c>
@@ -9139,7 +9138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>422105</v>
       </c>
@@ -9162,7 +9161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>422120</v>
       </c>
@@ -9185,7 +9184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>422125</v>
       </c>
@@ -9208,7 +9207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>422315</v>
       </c>
@@ -9231,7 +9230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>423105</v>
       </c>
@@ -9254,7 +9253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>510105</v>
       </c>
@@ -9277,7 +9276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>510305</v>
       </c>
@@ -9300,7 +9299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>510310</v>
       </c>
@@ -9323,7 +9322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>516805</v>
       </c>
@@ -9346,7 +9345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>520105</v>
       </c>
@@ -9369,7 +9368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>520110</v>
       </c>
@@ -9392,7 +9391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>521115</v>
       </c>
@@ -9415,7 +9414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>630110</v>
       </c>
@@ -9438,7 +9437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>710105</v>
       </c>
@@ -9461,7 +9460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>760405</v>
       </c>
@@ -9484,7 +9483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>810110</v>
       </c>
@@ -9507,7 +9506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>820210</v>
       </c>
@@ -9530,7 +9529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>860110</v>
       </c>
@@ -9553,7 +9552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>860115</v>
       </c>
@@ -9576,7 +9575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>910105</v>
       </c>
@@ -9599,7 +9598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>910115</v>
       </c>
@@ -9622,7 +9621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>950105</v>
       </c>
@@ -9645,7 +9644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>950110</v>
       </c>
@@ -9668,7 +9667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>950205</v>
       </c>
@@ -9691,7 +9690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>950305</v>
       </c>
@@ -9714,7 +9713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>992205</v>
       </c>
@@ -9747,11 +9746,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G352" xr:uid="{CCD02064-7416-4918-B4F4-C6A329ED0580}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G352">
       <sortCondition ref="G1:G352"/>
     </sortState>

</xml_diff>